<commit_message>
Implement UTF8 Encoding to open and save paths
</commit_message>
<xml_diff>
--- a/ImageMagickSharp/ImageMagickCommands.xlsx
+++ b/ImageMagickSharp/ImageMagickCommands.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4257" uniqueCount="2710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4259" uniqueCount="2710">
   <si>
     <t>ClearMagickWand</t>
   </si>
@@ -13338,11 +13338,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G579"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D265" sqref="D265:E265"/>
+      <pane ySplit="5" topLeftCell="A319" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C334" sqref="C334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13404,7 +13405,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>433</v>
       </c>
@@ -13426,7 +13427,7 @@
         <v>BorderColor</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
         <v>507</v>
       </c>
@@ -13448,7 +13449,7 @@
         <v>BorderColor</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
         <v>420</v>
       </c>
@@ -13470,7 +13471,7 @@
         <v>ClearDrawingWand</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
         <v>434</v>
       </c>
@@ -13487,7 +13488,7 @@
         <v>ClipPath</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
         <v>508</v>
       </c>
@@ -13504,7 +13505,7 @@
         <v>ClipPath</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
         <v>435</v>
       </c>
@@ -13521,7 +13522,7 @@
         <v>ClipRule</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
         <v>509</v>
       </c>
@@ -13538,7 +13539,7 @@
         <v>ClipRule</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
         <v>436</v>
       </c>
@@ -13555,7 +13556,7 @@
         <v>ClipUnits</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
         <v>510</v>
       </c>
@@ -13572,7 +13573,7 @@
         <v>ClipUnits</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14">
         <v>421</v>
       </c>
@@ -13594,7 +13595,7 @@
         <v>CloneDrawingWand</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14">
         <v>422</v>
       </c>
@@ -13616,7 +13617,7 @@
         <v>DestroyDrawingWand</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
         <v>423</v>
       </c>
@@ -13633,7 +13634,7 @@
         <v>DrawAffine</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14">
         <v>424</v>
       </c>
@@ -13655,7 +13656,7 @@
         <v>DrawAnnotation</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14">
         <v>425</v>
       </c>
@@ -13677,7 +13678,7 @@
         <v>DrawArc</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14">
         <v>426</v>
       </c>
@@ -13694,7 +13695,7 @@
         <v>DrawBezier</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14">
         <v>427</v>
       </c>
@@ -13716,7 +13717,7 @@
         <v>DrawCircle</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14">
         <v>428</v>
       </c>
@@ -13738,7 +13739,7 @@
         <v>DrawClearException</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14">
         <v>430</v>
       </c>
@@ -13760,7 +13761,7 @@
         <v>DrawColor</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14">
         <v>431</v>
       </c>
@@ -13777,7 +13778,7 @@
         <v>DrawComment</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14">
         <v>429</v>
       </c>
@@ -13799,7 +13800,7 @@
         <v>DrawComposite</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14">
         <v>432</v>
       </c>
@@ -13821,7 +13822,7 @@
         <v>DrawEllipse</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14">
         <v>470</v>
       </c>
@@ -13843,7 +13844,7 @@
         <v>DrawLine</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14">
         <v>471</v>
       </c>
@@ -13865,7 +13866,7 @@
         <v>DrawMatte</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14">
         <v>472</v>
       </c>
@@ -13882,7 +13883,7 @@
         <v>DrawPathClose</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14">
         <v>473</v>
       </c>
@@ -13899,7 +13900,7 @@
         <v>DrawPathCurveToAbsolute</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14">
         <v>475</v>
       </c>
@@ -13916,7 +13917,7 @@
         <v>DrawPathCurveToQuadraticBezierAbsolute</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14">
         <v>476</v>
       </c>
@@ -13933,7 +13934,7 @@
         <v>DrawPathCurveToQuadraticBezierRelative</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14">
         <v>477</v>
       </c>
@@ -13950,7 +13951,7 @@
         <v>DrawPathCurveToQuadraticBezierSmoothAbsolute</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14">
         <v>478</v>
       </c>
@@ -13967,7 +13968,7 @@
         <v>DrawPathCurveToQuadraticBezierSmoothRelative</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14">
         <v>474</v>
       </c>
@@ -13984,7 +13985,7 @@
         <v>DrawPathCurveToRelative</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14">
         <v>479</v>
       </c>
@@ -14001,7 +14002,7 @@
         <v>DrawPathCurveToSmoothAbsolute</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14">
         <v>480</v>
       </c>
@@ -14018,7 +14019,7 @@
         <v>DrawPathCurveToSmoothRelative</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14">
         <v>481</v>
       </c>
@@ -14035,7 +14036,7 @@
         <v>DrawPathEllipticArcAbsolute</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14">
         <v>482</v>
       </c>
@@ -14052,7 +14053,7 @@
         <v>DrawPathEllipticArcRelative</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14">
         <v>483</v>
       </c>
@@ -14069,7 +14070,7 @@
         <v>DrawPathFinish</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14">
         <v>484</v>
       </c>
@@ -14086,7 +14087,7 @@
         <v>DrawPathLineToAbsolute</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14">
         <v>486</v>
       </c>
@@ -14103,7 +14104,7 @@
         <v>DrawPathLineToHorizontalAbsolute</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14">
         <v>487</v>
       </c>
@@ -14120,7 +14121,7 @@
         <v>DrawPathLineToHorizontalRelative</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14">
         <v>485</v>
       </c>
@@ -14137,7 +14138,7 @@
         <v>DrawPathLineToRelative</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14">
         <v>488</v>
       </c>
@@ -14154,7 +14155,7 @@
         <v>DrawPathLineToVerticalAbsolute</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14">
         <v>489</v>
       </c>
@@ -14171,7 +14172,7 @@
         <v>DrawPathLineToVerticalRelative</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14">
         <v>490</v>
       </c>
@@ -14188,7 +14189,7 @@
         <v>DrawPathMoveToAbsolute</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14">
         <v>491</v>
       </c>
@@ -14205,7 +14206,7 @@
         <v>DrawPathMoveToRelative</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14">
         <v>492</v>
       </c>
@@ -14222,7 +14223,7 @@
         <v>DrawPathStart</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14">
         <v>493</v>
       </c>
@@ -14239,7 +14240,7 @@
         <v>DrawPoint</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="14">
         <v>494</v>
       </c>
@@ -14256,7 +14257,7 @@
         <v>DrawPolygon</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14">
         <v>495</v>
       </c>
@@ -14273,7 +14274,7 @@
         <v>DrawPolyline</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="14">
         <v>496</v>
       </c>
@@ -14290,7 +14291,7 @@
         <v>DrawPopClipPath</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14">
         <v>497</v>
       </c>
@@ -14307,7 +14308,7 @@
         <v>DrawPopDefs</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14">
         <v>498</v>
       </c>
@@ -14324,7 +14325,7 @@
         <v>DrawPopPattern</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14">
         <v>499</v>
       </c>
@@ -14341,7 +14342,7 @@
         <v>DrawPushClipPath</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14">
         <v>500</v>
       </c>
@@ -14358,7 +14359,7 @@
         <v>DrawPushDefs</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14">
         <v>501</v>
       </c>
@@ -14375,7 +14376,7 @@
         <v>DrawPushPattern</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14">
         <v>502</v>
       </c>
@@ -14397,7 +14398,7 @@
         <v>DrawRectangle</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14">
         <v>503</v>
       </c>
@@ -14419,7 +14420,7 @@
         <v>DrawResetVectorGraphics</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14">
         <v>504</v>
       </c>
@@ -14441,7 +14442,7 @@
         <v>DrawRotate</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14">
         <v>505</v>
       </c>
@@ -14463,7 +14464,7 @@
         <v>DrawRoundRectangle</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="14">
         <v>506</v>
       </c>
@@ -14485,7 +14486,7 @@
         <v>DrawScale</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="14">
         <v>544</v>
       </c>
@@ -14507,7 +14508,7 @@
         <v>DrawSkewX</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="14">
         <v>545</v>
       </c>
@@ -14529,7 +14530,7 @@
         <v>DrawSkewY</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14">
         <v>546</v>
       </c>
@@ -14551,7 +14552,7 @@
         <v>DrawTranslate</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="14">
         <v>437</v>
       </c>
@@ -14573,7 +14574,7 @@
         <v>Exception</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="14">
         <v>438</v>
       </c>
@@ -14595,7 +14596,7 @@
         <v>ExceptionType</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="14">
         <v>439</v>
       </c>
@@ -14617,7 +14618,7 @@
         <v>FillColor</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14">
         <v>511</v>
       </c>
@@ -14639,7 +14640,7 @@
         <v>FillColor</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="14">
         <v>440</v>
       </c>
@@ -14661,7 +14662,7 @@
         <v>FillOpacity</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="14">
         <v>512</v>
       </c>
@@ -14683,7 +14684,7 @@
         <v>FillOpacity</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="14">
         <v>515</v>
       </c>
@@ -14700,7 +14701,7 @@
         <v>FillPatternURL</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="14">
         <v>441</v>
       </c>
@@ -14717,7 +14718,7 @@
         <v>FillRule</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="14">
         <v>516</v>
       </c>
@@ -14734,7 +14735,7 @@
         <v>FillRule</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="14">
         <v>442</v>
       </c>
@@ -14756,7 +14757,7 @@
         <v>Font</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="14">
         <v>517</v>
       </c>
@@ -14778,7 +14779,7 @@
         <v>Font</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="14">
         <v>443</v>
       </c>
@@ -14800,7 +14801,7 @@
         <v>FontFamily</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="14">
         <v>518</v>
       </c>
@@ -14822,7 +14823,7 @@
         <v>FontFamily</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="14">
         <v>444</v>
       </c>
@@ -14844,7 +14845,7 @@
         <v>FontResolution</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="14">
         <v>513</v>
       </c>
@@ -14866,7 +14867,7 @@
         <v>FontResolution</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="14">
         <v>445</v>
       </c>
@@ -14888,7 +14889,7 @@
         <v>FontSize</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="14">
         <v>519</v>
       </c>
@@ -14910,7 +14911,7 @@
         <v>FontSize</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="14">
         <v>446</v>
       </c>
@@ -14932,7 +14933,7 @@
         <v>FontStretch</v>
       </c>
     </row>
-    <row r="85" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="14">
         <v>520</v>
       </c>
@@ -14954,7 +14955,7 @@
         <v>FontStretch</v>
       </c>
     </row>
-    <row r="86" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="14">
         <v>447</v>
       </c>
@@ -14976,7 +14977,7 @@
         <v>FontStyle</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="14">
         <v>521</v>
       </c>
@@ -14998,7 +14999,7 @@
         <v>FontStyle</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="14">
         <v>448</v>
       </c>
@@ -15020,7 +15021,7 @@
         <v>FontWeight</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="14">
         <v>522</v>
       </c>
@@ -15042,7 +15043,7 @@
         <v>FontWeight</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="14">
         <v>449</v>
       </c>
@@ -15064,7 +15065,7 @@
         <v>Gravity</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="14">
         <v>523</v>
       </c>
@@ -15086,7 +15087,7 @@
         <v>Gravity</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="14">
         <v>548</v>
       </c>
@@ -15103,7 +15104,7 @@
         <v>IsDrawingWand</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="14">
         <v>549</v>
       </c>
@@ -15125,7 +15126,7 @@
         <v>NewDrawingWand</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="14">
         <v>450</v>
       </c>
@@ -15147,7 +15148,7 @@
         <v>Opacity</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="14">
         <v>514</v>
       </c>
@@ -15169,7 +15170,7 @@
         <v>Opacity</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="14">
         <v>550</v>
       </c>
@@ -15186,7 +15187,7 @@
         <v>PeekDrawingWand</v>
       </c>
     </row>
-    <row r="97" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="14">
         <v>551</v>
       </c>
@@ -15203,7 +15204,7 @@
         <v>PopDrawingWand</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="14">
         <v>552</v>
       </c>
@@ -15220,7 +15221,7 @@
         <v>PushDrawingWand</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="14">
         <v>451</v>
       </c>
@@ -15242,7 +15243,7 @@
         <v>StrokeAntialias</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="14">
         <v>526</v>
       </c>
@@ -15264,7 +15265,7 @@
         <v>StrokeAntialias</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="14">
         <v>452</v>
       </c>
@@ -15286,7 +15287,7 @@
         <v>StrokeColor</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="14">
         <v>524</v>
       </c>
@@ -15308,7 +15309,7 @@
         <v>StrokeColor</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="14">
         <v>453</v>
       </c>
@@ -15325,7 +15326,7 @@
         <v>StrokeDashArray</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="14">
         <v>527</v>
       </c>
@@ -15342,7 +15343,7 @@
         <v>StrokeDashArray</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="14">
         <v>454</v>
       </c>
@@ -15359,7 +15360,7 @@
         <v>StrokeDashOffset</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="14">
         <v>528</v>
       </c>
@@ -15376,7 +15377,7 @@
         <v>StrokeDashOffset</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="14">
         <v>455</v>
       </c>
@@ -15393,7 +15394,7 @@
         <v>StrokeLineCap</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="14">
         <v>529</v>
       </c>
@@ -15410,7 +15411,7 @@
         <v>StrokeLineCap</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="14">
         <v>456</v>
       </c>
@@ -15427,7 +15428,7 @@
         <v>StrokeLineJoin</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="14">
         <v>530</v>
       </c>
@@ -15444,7 +15445,7 @@
         <v>StrokeLineJoin</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="14">
         <v>457</v>
       </c>
@@ -15461,7 +15462,7 @@
         <v>StrokeMiterLimit</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="14">
         <v>531</v>
       </c>
@@ -15478,7 +15479,7 @@
         <v>StrokeMiterLimit</v>
       </c>
     </row>
-    <row r="113" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="14">
         <v>458</v>
       </c>
@@ -15500,7 +15501,7 @@
         <v>StrokeOpacity</v>
       </c>
     </row>
-    <row r="114" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="14">
         <v>532</v>
       </c>
@@ -15522,7 +15523,7 @@
         <v>StrokeOpacity</v>
       </c>
     </row>
-    <row r="115" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="14">
         <v>525</v>
       </c>
@@ -15539,7 +15540,7 @@
         <v>StrokePatternURL</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="14">
         <v>459</v>
       </c>
@@ -15561,7 +15562,7 @@
         <v>StrokeWidth</v>
       </c>
     </row>
-    <row r="117" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="14">
         <v>533</v>
       </c>
@@ -15583,7 +15584,7 @@
         <v>StrokeWidth</v>
       </c>
     </row>
-    <row r="118" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="14">
         <v>460</v>
       </c>
@@ -15605,7 +15606,7 @@
         <v>TextAlignment</v>
       </c>
     </row>
-    <row r="119" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="14">
         <v>534</v>
       </c>
@@ -15627,7 +15628,7 @@
         <v>TextAlignment</v>
       </c>
     </row>
-    <row r="120" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="14">
         <v>461</v>
       </c>
@@ -15649,7 +15650,7 @@
         <v>TextAntialias</v>
       </c>
     </row>
-    <row r="121" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="14">
         <v>535</v>
       </c>
@@ -15671,7 +15672,7 @@
         <v>TextAntialias</v>
       </c>
     </row>
-    <row r="122" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="14">
         <v>462</v>
       </c>
@@ -15688,7 +15689,7 @@
         <v>TextDecoration</v>
       </c>
     </row>
-    <row r="123" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="14">
         <v>536</v>
       </c>
@@ -15705,7 +15706,7 @@
         <v>TextDecoration</v>
       </c>
     </row>
-    <row r="124" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="14">
         <v>463</v>
       </c>
@@ -15722,7 +15723,7 @@
         <v>TextDirection</v>
       </c>
     </row>
-    <row r="125" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="14">
         <v>537</v>
       </c>
@@ -15739,7 +15740,7 @@
         <v>TextDirection</v>
       </c>
     </row>
-    <row r="126" spans="1:7" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" s="19" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="14">
         <v>464</v>
       </c>
@@ -15756,7 +15757,7 @@
         <v>TextEncoding</v>
       </c>
     </row>
-    <row r="127" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="14">
         <v>538</v>
       </c>
@@ -15773,7 +15774,7 @@
         <v>TextEncoding</v>
       </c>
     </row>
-    <row r="128" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="14">
         <v>466</v>
       </c>
@@ -15790,7 +15791,7 @@
         <v>TextInterlineSpacing</v>
       </c>
     </row>
-    <row r="129" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="14">
         <v>540</v>
       </c>
@@ -15807,7 +15808,7 @@
         <v>TextInterlineSpacing</v>
       </c>
     </row>
-    <row r="130" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="14">
         <v>467</v>
       </c>
@@ -15824,7 +15825,7 @@
         <v>TextInterwordSpacing</v>
       </c>
     </row>
-    <row r="131" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="14">
         <v>541</v>
       </c>
@@ -15841,7 +15842,7 @@
         <v>TextInterwordSpacing</v>
       </c>
     </row>
-    <row r="132" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="14">
         <v>465</v>
       </c>
@@ -15858,7 +15859,7 @@
         <v>TextKerning</v>
       </c>
     </row>
-    <row r="133" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="14">
         <v>539</v>
       </c>
@@ -15875,7 +15876,7 @@
         <v>TextKerning</v>
       </c>
     </row>
-    <row r="134" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="14">
         <v>469</v>
       </c>
@@ -15897,7 +15898,7 @@
         <v>TextUnderColor</v>
       </c>
     </row>
-    <row r="135" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="14">
         <v>542</v>
       </c>
@@ -15919,7 +15920,7 @@
         <v>TextUnderColor</v>
       </c>
     </row>
-    <row r="136" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="14">
         <v>468</v>
       </c>
@@ -15941,7 +15942,7 @@
         <v>VectorGraphics</v>
       </c>
     </row>
-    <row r="137" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="14">
         <v>543</v>
       </c>
@@ -15963,7 +15964,7 @@
         <v>VectorGraphics</v>
       </c>
     </row>
-    <row r="138" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="14">
         <v>547</v>
       </c>
@@ -19397,10 +19398,15 @@
       <c r="B326" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C326" s="13" t="s">
+      <c r="C326" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D326" s="19"/>
+      <c r="D326" s="16" t="s">
+        <v>556</v>
+      </c>
+      <c r="E326" s="13" t="s">
+        <v>571</v>
+      </c>
       <c r="F326" s="17"/>
       <c r="G326" s="13" t="str">
         <f t="shared" ref="G326:G389" si="5">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(C326,"PixelSet",""),"PixelGet",""),"DrawSet",""),"DrawGet",""),"MagickSet",""),"MagickGet","")</f>
@@ -20778,7 +20784,7 @@
         <v>Use MagickBrightnessContrastImage</v>
       </c>
     </row>
-    <row r="401" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401" s="14">
         <v>28</v>
       </c>
@@ -20800,7 +20806,7 @@
         <v>Antialias</v>
       </c>
     </row>
-    <row r="402" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402" s="14">
         <v>66</v>
       </c>
@@ -20822,7 +20828,7 @@
         <v>Antialias</v>
       </c>
     </row>
-    <row r="403" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403" s="14">
         <v>29</v>
       </c>
@@ -20844,7 +20850,7 @@
         <v>BackgroundColor</v>
       </c>
     </row>
-    <row r="404" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404" s="14">
         <v>67</v>
       </c>
@@ -20866,7 +20872,7 @@
         <v>BackgroundColor</v>
       </c>
     </row>
-    <row r="405" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405" s="14">
         <v>30</v>
       </c>
@@ -20884,7 +20890,7 @@
         <v>Colorspace</v>
       </c>
     </row>
-    <row r="406" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" s="14">
         <v>68</v>
       </c>
@@ -20902,7 +20908,7 @@
         <v>Colorspace</v>
       </c>
     </row>
-    <row r="407" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407" s="14">
         <v>31</v>
       </c>
@@ -20920,7 +20926,7 @@
         <v>Compression</v>
       </c>
     </row>
-    <row r="408" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408" s="14">
         <v>69</v>
       </c>
@@ -20938,7 +20944,7 @@
         <v>Compression</v>
       </c>
     </row>
-    <row r="409" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409" s="14">
         <v>32</v>
       </c>
@@ -20956,7 +20962,7 @@
         <v>CompressionQuality</v>
       </c>
     </row>
-    <row r="410" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410" s="14">
         <v>70</v>
       </c>
@@ -20974,7 +20980,7 @@
         <v>CompressionQuality</v>
       </c>
     </row>
-    <row r="411" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A411" s="14">
         <v>33</v>
       </c>
@@ -20992,7 +20998,7 @@
         <v>Copyright</v>
       </c>
     </row>
-    <row r="412" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412" s="14">
         <v>71</v>
       </c>
@@ -21010,7 +21016,7 @@
         <v>Depth</v>
       </c>
     </row>
-    <row r="413" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413" s="14">
         <v>72</v>
       </c>
@@ -21028,7 +21034,7 @@
         <v>Extract</v>
       </c>
     </row>
-    <row r="414" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414" s="14">
         <v>34</v>
       </c>
@@ -21046,7 +21052,7 @@
         <v>Filename</v>
       </c>
     </row>
-    <row r="415" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415" s="14">
         <v>73</v>
       </c>
@@ -21064,7 +21070,7 @@
         <v>Filename</v>
       </c>
     </row>
-    <row r="416" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416" s="14">
         <v>35</v>
       </c>
@@ -21086,7 +21092,7 @@
         <v>Font</v>
       </c>
     </row>
-    <row r="417" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A417" s="14">
         <v>74</v>
       </c>
@@ -21108,7 +21114,7 @@
         <v>Font</v>
       </c>
     </row>
-    <row r="418" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418" s="14">
         <v>36</v>
       </c>
@@ -21126,7 +21132,7 @@
         <v>Format</v>
       </c>
     </row>
-    <row r="419" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419" s="14">
         <v>75</v>
       </c>
@@ -21143,7 +21149,7 @@
         <v>Format</v>
       </c>
     </row>
-    <row r="420" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420" s="14">
         <v>37</v>
       </c>
@@ -21165,7 +21171,7 @@
         <v>Gravity</v>
       </c>
     </row>
-    <row r="421" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421" s="14">
         <v>76</v>
       </c>
@@ -21187,7 +21193,7 @@
         <v>Gravity</v>
       </c>
     </row>
-    <row r="422" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422" s="14">
         <v>38</v>
       </c>
@@ -21205,7 +21211,7 @@
         <v>HomeURL</v>
       </c>
     </row>
-    <row r="423" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A423" s="14">
         <v>39</v>
       </c>
@@ -21223,7 +21229,7 @@
         <v>ImageArtifact</v>
       </c>
     </row>
-    <row r="424" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A424" s="14">
         <v>77</v>
       </c>
@@ -21240,7 +21246,7 @@
         <v>ImageArtifact</v>
       </c>
     </row>
-    <row r="425" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A425" s="14">
         <v>40</v>
       </c>
@@ -21258,7 +21264,7 @@
         <v>ImageArtifacts</v>
       </c>
     </row>
-    <row r="426" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426" s="14">
         <v>41</v>
       </c>
@@ -21276,7 +21282,7 @@
         <v>ImageProfile</v>
       </c>
     </row>
-    <row r="427" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A427" s="14">
         <v>78</v>
       </c>
@@ -21293,7 +21299,7 @@
         <v>ImageProfile</v>
       </c>
     </row>
-    <row r="428" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A428" s="14">
         <v>42</v>
       </c>
@@ -21311,7 +21317,7 @@
         <v>ImageProfiles</v>
       </c>
     </row>
-    <row r="429" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A429" s="14">
         <v>44</v>
       </c>
@@ -21329,7 +21335,7 @@
         <v>ImageProperties</v>
       </c>
     </row>
-    <row r="430" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A430" s="14">
         <v>43</v>
       </c>
@@ -21347,7 +21353,7 @@
         <v>ImageProperty</v>
       </c>
     </row>
-    <row r="431" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A431" s="14">
         <v>79</v>
       </c>
@@ -21364,7 +21370,7 @@
         <v>ImageProperty</v>
       </c>
     </row>
-    <row r="432" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A432" s="14">
         <v>45</v>
       </c>
@@ -21382,7 +21388,7 @@
         <v>InterlaceScheme</v>
       </c>
     </row>
-    <row r="433" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A433" s="14">
         <v>80</v>
       </c>
@@ -21399,7 +21405,7 @@
         <v>InterlaceScheme</v>
       </c>
     </row>
-    <row r="434" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A434" s="14">
         <v>46</v>
       </c>
@@ -21417,7 +21423,7 @@
         <v>InterpolateMethod</v>
       </c>
     </row>
-    <row r="435" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A435" s="14">
         <v>81</v>
       </c>
@@ -21434,7 +21440,7 @@
         <v>InterpolateMethod</v>
       </c>
     </row>
-    <row r="436" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A436" s="14">
         <v>25</v>
       </c>
@@ -21451,7 +21457,7 @@
         <v>MagickDeleteImageArtifact</v>
       </c>
     </row>
-    <row r="437" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A437" s="14">
         <v>26</v>
       </c>
@@ -21468,7 +21474,7 @@
         <v>MagickDeleteImageProperty</v>
       </c>
     </row>
-    <row r="438" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A438" s="14">
         <v>27</v>
       </c>
@@ -21486,7 +21492,7 @@
         <v>MagickDeleteOption</v>
       </c>
     </row>
-    <row r="439" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A439" s="14">
         <v>64</v>
       </c>
@@ -21504,7 +21510,7 @@
         <v>MagickProfileImage</v>
       </c>
     </row>
-    <row r="440" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A440" s="14">
         <v>65</v>
       </c>
@@ -21522,7 +21528,7 @@
         <v>MagickRemoveImageProfile</v>
       </c>
     </row>
-    <row r="441" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A441" s="14">
         <v>47</v>
       </c>
@@ -21540,7 +21546,7 @@
         <v>Option</v>
       </c>
     </row>
-    <row r="442" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A442" s="14">
         <v>82</v>
       </c>
@@ -21557,7 +21563,7 @@
         <v>Option</v>
       </c>
     </row>
-    <row r="443" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A443" s="14">
         <v>48</v>
       </c>
@@ -21575,7 +21581,7 @@
         <v>Options</v>
       </c>
     </row>
-    <row r="444" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A444" s="14">
         <v>49</v>
       </c>
@@ -21593,7 +21599,7 @@
         <v>Orientation</v>
       </c>
     </row>
-    <row r="445" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A445" s="14">
         <v>83</v>
       </c>
@@ -21610,7 +21616,7 @@
         <v>Orientation</v>
       </c>
     </row>
-    <row r="446" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A446" s="14">
         <v>50</v>
       </c>
@@ -21628,7 +21634,7 @@
         <v>PackageName</v>
       </c>
     </row>
-    <row r="447" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A447" s="14">
         <v>51</v>
       </c>
@@ -21650,7 +21656,7 @@
         <v>Page</v>
       </c>
     </row>
-    <row r="448" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448" s="14">
         <v>84</v>
       </c>
@@ -21672,7 +21678,7 @@
         <v>Page</v>
       </c>
     </row>
-    <row r="449" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449" s="14">
         <v>85</v>
       </c>
@@ -21689,7 +21695,7 @@
         <v>Passphrase</v>
       </c>
     </row>
-    <row r="450" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" s="14">
         <v>52</v>
       </c>
@@ -21711,7 +21717,7 @@
         <v>Pointsize</v>
       </c>
     </row>
-    <row r="451" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" s="14">
         <v>86</v>
       </c>
@@ -21733,7 +21739,7 @@
         <v>Pointsize</v>
       </c>
     </row>
-    <row r="452" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" s="14">
         <v>87</v>
       </c>
@@ -21750,7 +21756,7 @@
         <v>ProgressMonitor</v>
       </c>
     </row>
-    <row r="453" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A453" s="14">
         <v>53</v>
       </c>
@@ -21770,7 +21776,7 @@
         <v>QuantumDepth</v>
       </c>
     </row>
-    <row r="454" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A454" s="14">
         <v>54</v>
       </c>
@@ -21788,7 +21794,7 @@
         <v>QuantumRange</v>
       </c>
     </row>
-    <row r="455" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A455" s="14">
         <v>55</v>
       </c>
@@ -21806,7 +21812,7 @@
         <v>ReleaseDate</v>
       </c>
     </row>
-    <row r="456" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A456" s="14">
         <v>56</v>
       </c>
@@ -21824,7 +21830,7 @@
         <v>Resolution</v>
       </c>
     </row>
-    <row r="457" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A457" s="14">
         <v>89</v>
       </c>
@@ -21841,7 +21847,7 @@
         <v>Resolution</v>
       </c>
     </row>
-    <row r="458" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A458" s="14">
         <v>57</v>
       </c>
@@ -21859,7 +21865,7 @@
         <v>Resource</v>
       </c>
     </row>
-    <row r="459" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A459" s="14">
         <v>58</v>
       </c>
@@ -21877,7 +21883,7 @@
         <v>ResourceLimit</v>
       </c>
     </row>
-    <row r="460" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A460" s="14">
         <v>88</v>
       </c>
@@ -21894,7 +21900,7 @@
         <v>ResourceLimit</v>
       </c>
     </row>
-    <row r="461" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461" s="14">
         <v>59</v>
       </c>
@@ -21912,7 +21918,7 @@
         <v>SamplingFactors</v>
       </c>
     </row>
-    <row r="462" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A462" s="14">
         <v>90</v>
       </c>
@@ -21929,7 +21935,7 @@
         <v>SamplingFactors</v>
       </c>
     </row>
-    <row r="463" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A463" s="14">
         <v>60</v>
       </c>
@@ -21951,7 +21957,7 @@
         <v>Size</v>
       </c>
     </row>
-    <row r="464" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A464" s="14">
         <v>91</v>
       </c>
@@ -21973,7 +21979,7 @@
         <v>Size</v>
       </c>
     </row>
-    <row r="465" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A465" s="14">
         <v>61</v>
       </c>
@@ -21991,7 +21997,7 @@
         <v>SizeOffset</v>
       </c>
     </row>
-    <row r="466" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A466" s="14">
         <v>92</v>
       </c>
@@ -22009,7 +22015,7 @@
         <v>SizeOffset</v>
       </c>
     </row>
-    <row r="467" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A467" s="14">
         <v>62</v>
       </c>
@@ -22027,7 +22033,7 @@
         <v>Type</v>
       </c>
     </row>
-    <row r="468" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A468" s="14">
         <v>93</v>
       </c>
@@ -22045,7 +22051,7 @@
         <v>Type</v>
       </c>
     </row>
-    <row r="469" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A469" s="14">
         <v>63</v>
       </c>
@@ -22069,7 +22075,7 @@
         <v>Version</v>
       </c>
     </row>
-    <row r="470" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A470" s="14">
         <v>1</v>
       </c>
@@ -22093,7 +22099,7 @@
         <v>ClearMagickWand</v>
       </c>
     </row>
-    <row r="471" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A471" s="14">
         <v>2</v>
       </c>
@@ -22115,7 +22121,7 @@
         <v>CloneMagickWand</v>
       </c>
     </row>
-    <row r="472" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A472" s="14">
         <v>3</v>
       </c>
@@ -22139,7 +22145,7 @@
         <v>DestroyMagickWand</v>
       </c>
     </row>
-    <row r="473" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A473" s="14">
         <v>6</v>
       </c>
@@ -22163,7 +22169,7 @@
         <v>Exception</v>
       </c>
     </row>
-    <row r="474" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A474" s="14">
         <v>7</v>
       </c>
@@ -22187,7 +22193,7 @@
         <v>ExceptionType</v>
       </c>
     </row>
-    <row r="475" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A475" s="14">
         <v>17</v>
       </c>
@@ -22209,7 +22215,7 @@
         <v>FirstIterator</v>
       </c>
     </row>
-    <row r="476" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A476" s="14">
         <v>4</v>
       </c>
@@ -22233,7 +22239,7 @@
         <v>IsMagickWand</v>
       </c>
     </row>
-    <row r="477" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A477" s="14">
         <v>24</v>
       </c>
@@ -22257,7 +22263,7 @@
         <v>IsMagickWandInstantiated</v>
       </c>
     </row>
-    <row r="478" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A478" s="14">
         <v>8</v>
       </c>
@@ -22279,7 +22285,7 @@
         <v>IteratorIndex</v>
       </c>
     </row>
-    <row r="479" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A479" s="14">
         <v>18</v>
       </c>
@@ -22301,7 +22307,7 @@
         <v>IteratorIndex</v>
       </c>
     </row>
-    <row r="480" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A480" s="14">
         <v>19</v>
       </c>
@@ -22323,7 +22329,7 @@
         <v>LastIterator</v>
       </c>
     </row>
-    <row r="481" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A481" s="14">
         <v>5</v>
       </c>
@@ -22347,7 +22353,7 @@
         <v>MagickClearException</v>
       </c>
     </row>
-    <row r="482" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A482" s="14">
         <v>9</v>
       </c>
@@ -22364,7 +22370,7 @@
         <v>MagickQueryConfigureOption</v>
       </c>
     </row>
-    <row r="483" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A483" s="14">
         <v>10</v>
       </c>
@@ -22381,7 +22387,7 @@
         <v>MagickQueryConfigureOptions</v>
       </c>
     </row>
-    <row r="484" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A484" s="14">
         <v>11</v>
       </c>
@@ -22398,7 +22404,7 @@
         <v>MagickQueryFontMetrics</v>
       </c>
     </row>
-    <row r="485" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A485" s="14">
         <v>13</v>
       </c>
@@ -22415,7 +22421,7 @@
         <v>MagickQueryFonts</v>
       </c>
     </row>
-    <row r="486" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A486" s="14">
         <v>14</v>
       </c>
@@ -22432,7 +22438,7 @@
         <v>MagickQueryFormats</v>
       </c>
     </row>
-    <row r="487" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A487" s="14">
         <v>12</v>
       </c>
@@ -22449,7 +22455,7 @@
         <v>MagickQueryMultilineFontMetrics</v>
       </c>
     </row>
-    <row r="488" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A488" s="14">
         <v>15</v>
       </c>
@@ -22473,7 +22479,7 @@
         <v>MagickRelinquishMemory</v>
       </c>
     </row>
-    <row r="489" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A489" s="14">
         <v>16</v>
       </c>
@@ -22495,7 +22501,7 @@
         <v>MagickResetIterator</v>
       </c>
     </row>
-    <row r="490" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A490" s="14">
         <v>20</v>
       </c>
@@ -22519,7 +22525,7 @@
         <v>MagickWandGenesis</v>
       </c>
     </row>
-    <row r="491" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A491" s="14">
         <v>21</v>
       </c>
@@ -22543,7 +22549,7 @@
         <v>MagickWandTerminus</v>
       </c>
     </row>
-    <row r="492" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A492" s="14">
         <v>22</v>
       </c>
@@ -22565,7 +22571,7 @@
         <v>NewMagickWand</v>
       </c>
     </row>
-    <row r="493" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A493" s="14">
         <v>23</v>
       </c>
@@ -22582,7 +22588,7 @@
         <v>NewMagickWandFromImage</v>
       </c>
     </row>
-    <row r="494" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A494" s="14">
         <v>571</v>
       </c>
@@ -22604,7 +22610,7 @@
         <v>MagickCommandGenesis</v>
       </c>
     </row>
-    <row r="495" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A495" s="14">
         <v>553</v>
       </c>
@@ -22626,7 +22632,7 @@
         <v>ClearPixelIterator</v>
       </c>
     </row>
-    <row r="496" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A496" s="14">
         <v>554</v>
       </c>
@@ -22648,7 +22654,7 @@
         <v>ClonePixelIterator</v>
       </c>
     </row>
-    <row r="497" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A497" s="14">
         <v>560</v>
       </c>
@@ -22670,7 +22676,7 @@
         <v>CurrentIteratorRow</v>
       </c>
     </row>
-    <row r="498" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A498" s="14">
         <v>555</v>
       </c>
@@ -22692,7 +22698,7 @@
         <v>DestroyPixelIterator</v>
       </c>
     </row>
-    <row r="499" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A499" s="14">
         <v>567</v>
       </c>
@@ -22714,7 +22720,7 @@
         <v>FirstIteratorRow</v>
       </c>
     </row>
-    <row r="500" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A500" s="14">
         <v>556</v>
       </c>
@@ -22736,7 +22742,7 @@
         <v>IsPixelIterator</v>
       </c>
     </row>
-    <row r="501" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A501" s="14">
         <v>561</v>
       </c>
@@ -22758,7 +22764,7 @@
         <v>IteratorException</v>
       </c>
     </row>
-    <row r="502" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A502" s="14">
         <v>562</v>
       </c>
@@ -22780,7 +22786,7 @@
         <v>IteratorExceptionType</v>
       </c>
     </row>
-    <row r="503" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A503" s="14">
         <v>563</v>
       </c>
@@ -22802,7 +22808,7 @@
         <v>IteratorRow</v>
       </c>
     </row>
-    <row r="504" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A504" s="14">
         <v>568</v>
       </c>
@@ -22824,7 +22830,7 @@
         <v>IteratorRow</v>
       </c>
     </row>
-    <row r="505" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A505" s="14">
         <v>569</v>
       </c>
@@ -22846,7 +22852,7 @@
         <v>LastIteratorRow</v>
       </c>
     </row>
-    <row r="506" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A506" s="14">
         <v>557</v>
       </c>
@@ -22868,7 +22874,7 @@
         <v>NewPixelIterator</v>
       </c>
     </row>
-    <row r="507" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A507" s="14">
         <v>559</v>
       </c>
@@ -22890,7 +22896,7 @@
         <v>NewPixelRegionIterator</v>
       </c>
     </row>
-    <row r="508" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A508" s="14">
         <v>564</v>
       </c>
@@ -22912,7 +22918,7 @@
         <v>NextIteratorRow</v>
       </c>
     </row>
-    <row r="509" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A509" s="14">
         <v>558</v>
       </c>
@@ -22934,7 +22940,7 @@
         <v>PixelClearIteratorException</v>
       </c>
     </row>
-    <row r="510" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A510" s="14">
         <v>566</v>
       </c>
@@ -22956,7 +22962,7 @@
         <v>PixelResetIterator</v>
       </c>
     </row>
-    <row r="511" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A511" s="14">
         <v>570</v>
       </c>
@@ -22978,7 +22984,7 @@
         <v>PixelSyncIterator</v>
       </c>
     </row>
-    <row r="512" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A512" s="14">
         <v>565</v>
       </c>
@@ -23000,7 +23006,7 @@
         <v>PreviousIteratorRow</v>
       </c>
     </row>
-    <row r="513" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A513" s="14">
         <v>366</v>
       </c>
@@ -23022,7 +23028,7 @@
         <v>Alpha</v>
       </c>
     </row>
-    <row r="514" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A514" s="14">
         <v>394</v>
       </c>
@@ -23044,7 +23050,7 @@
         <v>Alpha</v>
       </c>
     </row>
-    <row r="515" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A515" s="14">
         <v>367</v>
       </c>
@@ -23061,7 +23067,7 @@
         <v>AlphaQuantum</v>
       </c>
     </row>
-    <row r="516" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A516" s="14">
         <v>395</v>
       </c>
@@ -23078,7 +23084,7 @@
         <v>AlphaQuantum</v>
       </c>
     </row>
-    <row r="517" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A517" s="14">
         <v>368</v>
       </c>
@@ -23095,7 +23101,7 @@
         <v>Black</v>
       </c>
     </row>
-    <row r="518" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A518" s="14">
         <v>396</v>
       </c>
@@ -23112,7 +23118,7 @@
         <v>Black</v>
       </c>
     </row>
-    <row r="519" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A519" s="14">
         <v>369</v>
       </c>
@@ -23129,7 +23135,7 @@
         <v>BlackQuantum</v>
       </c>
     </row>
-    <row r="520" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A520" s="14">
         <v>397</v>
       </c>
@@ -23146,7 +23152,7 @@
         <v>BlackQuantum</v>
       </c>
     </row>
-    <row r="521" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A521" s="14">
         <v>370</v>
       </c>
@@ -23168,7 +23174,7 @@
         <v>Blue</v>
       </c>
     </row>
-    <row r="522" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A522" s="14">
         <v>398</v>
       </c>
@@ -23190,7 +23196,7 @@
         <v>Blue</v>
       </c>
     </row>
-    <row r="523" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A523" s="14">
         <v>371</v>
       </c>
@@ -23207,7 +23213,7 @@
         <v>BlueQuantum</v>
       </c>
     </row>
-    <row r="524" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A524" s="14">
         <v>399</v>
       </c>
@@ -23224,7 +23230,7 @@
         <v>BlueQuantum</v>
       </c>
     </row>
-    <row r="525" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A525" s="14">
         <v>356</v>
       </c>
@@ -23246,7 +23252,7 @@
         <v>ClearPixelWand</v>
       </c>
     </row>
-    <row r="526" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="526" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A526" s="14">
         <v>357</v>
       </c>
@@ -23268,7 +23274,7 @@
         <v>ClonePixelWand</v>
       </c>
     </row>
-    <row r="527" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="527" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A527" s="14">
         <v>358</v>
       </c>
@@ -23285,7 +23291,7 @@
         <v>ClonePixelWands</v>
       </c>
     </row>
-    <row r="528" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="528" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A528" s="14">
         <v>400</v>
       </c>
@@ -23307,7 +23313,7 @@
         <v>Color</v>
       </c>
     </row>
-    <row r="529" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A529" s="14">
         <v>373</v>
       </c>
@@ -23329,7 +23335,7 @@
         <v>ColorAsNormalizedString</v>
       </c>
     </row>
-    <row r="530" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A530" s="14">
         <v>372</v>
       </c>
@@ -23351,7 +23357,7 @@
         <v>ColorAsString</v>
       </c>
     </row>
-    <row r="531" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A531" s="14">
         <v>374</v>
       </c>
@@ -23368,7 +23374,7 @@
         <v>ColorCount</v>
       </c>
     </row>
-    <row r="532" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A532" s="14">
         <v>401</v>
       </c>
@@ -23385,7 +23391,7 @@
         <v>ColorCount</v>
       </c>
     </row>
-    <row r="533" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A533" s="14">
         <v>402</v>
       </c>
@@ -23402,7 +23408,7 @@
         <v>ColorFromWand</v>
       </c>
     </row>
-    <row r="534" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A534" s="14">
         <v>375</v>
       </c>
@@ -23419,7 +23425,7 @@
         <v>Cyan</v>
       </c>
     </row>
-    <row r="535" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A535" s="14">
         <v>403</v>
       </c>
@@ -23436,7 +23442,7 @@
         <v>Cyan</v>
       </c>
     </row>
-    <row r="536" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A536" s="14">
         <v>376</v>
       </c>
@@ -23453,7 +23459,7 @@
         <v>CyanQuantum</v>
       </c>
     </row>
-    <row r="537" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A537" s="14">
         <v>404</v>
       </c>
@@ -23470,7 +23476,7 @@
         <v>CyanQuantum</v>
       </c>
     </row>
-    <row r="538" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A538" s="14">
         <v>359</v>
       </c>
@@ -23487,7 +23493,7 @@
         <v>DestroyPixelWand</v>
       </c>
     </row>
-    <row r="539" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A539" s="14">
         <v>360</v>
       </c>
@@ -23509,7 +23515,7 @@
         <v>DestroyPixelWands</v>
       </c>
     </row>
-    <row r="540" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A540" s="14">
         <v>377</v>
       </c>
@@ -23531,7 +23537,7 @@
         <v>Exception</v>
       </c>
     </row>
-    <row r="541" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A541" s="14">
         <v>378</v>
       </c>
@@ -23553,7 +23559,7 @@
         <v>ExceptionType</v>
       </c>
     </row>
-    <row r="542" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A542" s="14">
         <v>379</v>
       </c>
@@ -23570,7 +23576,7 @@
         <v>Fuzz</v>
       </c>
     </row>
-    <row r="543" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A543" s="14">
         <v>405</v>
       </c>
@@ -23587,7 +23593,7 @@
         <v>Fuzz</v>
       </c>
     </row>
-    <row r="544" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A544" s="14">
         <v>380</v>
       </c>
@@ -23609,7 +23615,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="545" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="545" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A545" s="14">
         <v>406</v>
       </c>
@@ -23631,7 +23637,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="546" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A546" s="14">
         <v>381</v>
       </c>
@@ -23648,7 +23654,7 @@
         <v>GreenQuantum</v>
       </c>
     </row>
-    <row r="547" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A547" s="14">
         <v>407</v>
       </c>
@@ -23665,7 +23671,7 @@
         <v>GreenQuantum</v>
       </c>
     </row>
-    <row r="548" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A548" s="14">
         <v>382</v>
       </c>
@@ -23682,7 +23688,7 @@
         <v>HSL</v>
       </c>
     </row>
-    <row r="549" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="549" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A549" s="14">
         <v>408</v>
       </c>
@@ -23699,7 +23705,7 @@
         <v>HSL</v>
       </c>
     </row>
-    <row r="550" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A550" s="14">
         <v>383</v>
       </c>
@@ -23716,7 +23722,7 @@
         <v>Index</v>
       </c>
     </row>
-    <row r="551" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A551" s="14">
         <v>409</v>
       </c>
@@ -23733,7 +23739,7 @@
         <v>Index</v>
       </c>
     </row>
-    <row r="552" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="552" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A552" s="14">
         <v>362</v>
       </c>
@@ -23750,7 +23756,7 @@
         <v>IsPixelWand</v>
       </c>
     </row>
-    <row r="553" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A553" s="14">
         <v>361</v>
       </c>
@@ -23767,7 +23773,7 @@
         <v>IsPixelWandSimilar</v>
       </c>
     </row>
-    <row r="554" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A554" s="14">
         <v>384</v>
       </c>
@@ -23784,7 +23790,7 @@
         <v>Magenta</v>
       </c>
     </row>
-    <row r="555" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="555" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A555" s="14">
         <v>410</v>
       </c>
@@ -23801,7 +23807,7 @@
         <v>Magenta</v>
       </c>
     </row>
-    <row r="556" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="556" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A556" s="14">
         <v>385</v>
       </c>
@@ -23818,7 +23824,7 @@
         <v>MagentaQuantum</v>
       </c>
     </row>
-    <row r="557" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="557" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A557" s="14">
         <v>411</v>
       </c>
@@ -23835,7 +23841,7 @@
         <v>MagentaQuantum</v>
       </c>
     </row>
-    <row r="558" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A558" s="14">
         <v>386</v>
       </c>
@@ -23852,7 +23858,7 @@
         <v>MagickColor</v>
       </c>
     </row>
-    <row r="559" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A559" s="14">
         <v>412</v>
       </c>
@@ -23869,7 +23875,7 @@
         <v>MagickColor</v>
       </c>
     </row>
-    <row r="560" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="560" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A560" s="14">
         <v>363</v>
       </c>
@@ -23891,7 +23897,7 @@
         <v>NewPixelWand</v>
       </c>
     </row>
-    <row r="561" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A561" s="14">
         <v>364</v>
       </c>
@@ -23908,7 +23914,7 @@
         <v>NewPixelWands</v>
       </c>
     </row>
-    <row r="562" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A562" s="14">
         <v>387</v>
       </c>
@@ -23930,7 +23936,7 @@
         <v>Opacity</v>
       </c>
     </row>
-    <row r="563" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A563" s="14">
         <v>413</v>
       </c>
@@ -23952,7 +23958,7 @@
         <v>Opacity</v>
       </c>
     </row>
-    <row r="564" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A564" s="14">
         <v>388</v>
       </c>
@@ -23969,7 +23975,7 @@
         <v>OpacityQuantum</v>
       </c>
     </row>
-    <row r="565" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A565" s="14">
         <v>414</v>
       </c>
@@ -23986,7 +23992,7 @@
         <v>OpacityQuantum</v>
       </c>
     </row>
-    <row r="566" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A566" s="14">
         <v>365</v>
       </c>
@@ -24005,7 +24011,7 @@
         <v>PixelClearException</v>
       </c>
     </row>
-    <row r="567" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A567" s="14">
         <v>389</v>
       </c>
@@ -24022,7 +24028,7 @@
         <v>QuantumColor</v>
       </c>
     </row>
-    <row r="568" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A568" s="14">
         <v>415</v>
       </c>
@@ -24039,7 +24045,7 @@
         <v>QuantumColor</v>
       </c>
     </row>
-    <row r="569" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A569" s="14">
         <v>390</v>
       </c>
@@ -24061,7 +24067,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="570" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A570" s="14">
         <v>416</v>
       </c>
@@ -24083,7 +24089,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="571" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A571" s="14">
         <v>391</v>
       </c>
@@ -24100,7 +24106,7 @@
         <v>RedQuantum</v>
       </c>
     </row>
-    <row r="572" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A572" s="14">
         <v>417</v>
       </c>
@@ -24117,7 +24123,7 @@
         <v>RedQuantum</v>
       </c>
     </row>
-    <row r="573" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A573" s="14">
         <v>392</v>
       </c>
@@ -24134,7 +24140,7 @@
         <v>Yellow</v>
       </c>
     </row>
-    <row r="574" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A574" s="14">
         <v>418</v>
       </c>
@@ -24151,7 +24157,7 @@
         <v>Yellow</v>
       </c>
     </row>
-    <row r="575" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A575" s="14">
         <v>393</v>
       </c>
@@ -24168,7 +24174,7 @@
         <v>YellowQuantum</v>
       </c>
     </row>
-    <row r="576" spans="1:7" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:7" s="13" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A576" s="14">
         <v>419</v>
       </c>
@@ -24201,7 +24207,13 @@
       <c r="F579" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:G576"/>
+  <autoFilter ref="A5:G576">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Module magick-image Methods"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A6:G576">
     <sortCondition ref="B6:B576"/>
     <sortCondition ref="G6:G576"/>

</xml_diff>

<commit_message>
Code fix and added some functions
</commit_message>
<xml_diff>
--- a/ImageMagickSharp/ImageMagickCommands.xlsx
+++ b/ImageMagickSharp/ImageMagickCommands.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4259" uniqueCount="2710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4269" uniqueCount="2710">
   <si>
     <t>ClearMagickWand</t>
   </si>
@@ -13341,8 +13341,8 @@
   <dimension ref="A1:G579"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A508" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C334" sqref="C334"/>
+      <pane ySplit="5" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E142" sqref="E142:E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16049,10 +16049,15 @@
       <c r="B142" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C142" s="13" t="s">
+      <c r="C142" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D142" s="19"/>
+      <c r="D142" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E142" s="13" t="s">
+        <v>570</v>
+      </c>
       <c r="F142" s="17"/>
       <c r="G142" s="13" t="str">
         <f t="shared" si="2"/>
@@ -16066,10 +16071,15 @@
       <c r="B143" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C143" s="13" t="s">
+      <c r="C143" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="D143" s="19"/>
+      <c r="D143" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E143" s="13" t="s">
+        <v>570</v>
+      </c>
       <c r="F143" s="17"/>
       <c r="G143" s="13" t="str">
         <f t="shared" si="2"/>
@@ -16413,10 +16423,15 @@
       <c r="B162" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C162" s="13" t="s">
+      <c r="C162" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D162" s="19"/>
+      <c r="D162" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E162" s="13" t="s">
+        <v>571</v>
+      </c>
       <c r="F162" s="17"/>
       <c r="G162" s="13" t="str">
         <f t="shared" si="2"/>
@@ -16430,10 +16445,15 @@
       <c r="B163" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C163" s="13" t="s">
+      <c r="C163" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="D163" s="19"/>
+      <c r="D163" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E163" s="13" t="s">
+        <v>571</v>
+      </c>
       <c r="F163" s="17"/>
       <c r="G163" s="13" t="str">
         <f t="shared" si="2"/>
@@ -19380,10 +19400,15 @@
       <c r="B325" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C325" s="13" t="s">
+      <c r="C325" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="D325" s="19"/>
+      <c r="D325" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E325" s="13" t="s">
+        <v>571</v>
+      </c>
       <c r="F325" s="17"/>
       <c r="G325" s="13" t="str">
         <f t="shared" si="4"/>

</xml_diff>